<commit_message>
updated folders, updated customer seg
</commit_message>
<xml_diff>
--- a/Images.xlsx
+++ b/Images.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachid\Desktop\Market_Camp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EE4EF41-4004-4AA3-A8D6-EF896F391E18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051C8052-AD9F-4BF7-A268-7FB2580E0BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D0EB39B2-2CB9-4227-9FFD-7142CF857DC5}"/>
+    <workbookView xWindow="18636" yWindow="1308" windowWidth="8760" windowHeight="6000" activeTab="1" xr2:uid="{D0EB39B2-2CB9-4227-9FFD-7142CF857DC5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="D.Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="ML" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1109,6 +1110,646 @@
         <a:xfrm>
           <a:off x="4800600" y="23123237"/>
           <a:ext cx="3857143" cy="1152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>26194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>357626</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>115723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0117F4B-2541-4122-824F-365A69260B3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2651760" y="1306354"/>
+          <a:ext cx="3801866" cy="3564249"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Star: 5 Points 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDD556E7-C329-406A-AE77-13ED1735D6AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3985260" y="3672840"/>
+          <a:ext cx="182880" cy="205740"/>
+        </a:xfrm>
+        <a:prstGeom prst="star5">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>546408</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>177016</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FED8347-1385-4354-842D-793102214DD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1584960" y="5387340"/>
+          <a:ext cx="2619048" cy="1190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>468356</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D7A8BCB-F7FB-427F-80A6-5218D342B593}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4373880" y="5372100"/>
+          <a:ext cx="2190476" cy="1209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>510249</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>150349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9BAEA45-15E6-4715-B788-B41103972E38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6720840" y="5379720"/>
+          <a:ext cx="2323809" cy="1171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>84848</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>14897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{059F6F3B-FEEC-4BBA-9559-42E31AAC8027}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1600200" y="6598920"/>
+          <a:ext cx="7019048" cy="2742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>122933</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>138873</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0EA39C9-EBF9-466F-9FC7-D80A416BF481}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="9578340"/>
+          <a:ext cx="7133333" cy="1533333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>300068</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>85538</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{612241B9-A050-4122-94A7-B23FF4A55B7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1463040" y="11391900"/>
+          <a:ext cx="7371428" cy="1495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>147459</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>13141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2198EA03-9C7C-4609-8942-F45D7F37ED81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1463040" y="12908280"/>
+          <a:ext cx="9047619" cy="1552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>113400</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>178877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{238C685B-CC4B-43F0-8B56-A473874A1B18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1447800" y="14546580"/>
+          <a:ext cx="7200000" cy="1542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>497353</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>450665</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>65805</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8D9BCAF-A853-4B45-BEBB-4B99532F45D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1716553" y="16253460"/>
+          <a:ext cx="4220512" cy="4477785"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>5130</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>174769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B496B1-416D-4671-98B6-79AADA146D14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1424940" y="21122640"/>
+          <a:ext cx="4676190" cy="3923809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>16549</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>178587</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E99069A-7248-4CEA-9391-0C4C6BD7D625}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6217920" y="21183600"/>
+          <a:ext cx="4771429" cy="3866667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>513748</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>182385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECEDC60A-6271-45E4-9740-C59195E0E2C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10934700" y="21092160"/>
+          <a:ext cx="4819048" cy="3961905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1419,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF53098D-0567-46ED-904F-53C8C4E6A9CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="A96" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="Q129" sqref="Q129"/>
     </sheetView>
   </sheetViews>
@@ -1431,4 +2072,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2464488F-2CC8-4DB3-B98B-28995812AE4D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="Q140" sqref="Q140"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>